<commit_message>
TP#15397 Fix formatting, weight and unit were flipped on one row
</commit_message>
<xml_diff>
--- a/Code/ShipWorks.Tests.Integration/DataSources/FedExAll/US Exp Dom-Alcohol.xlsx
+++ b/Code/ShipWorks.Tests.Integration/DataSources/FedExAll/US Exp Dom-Alcohol.xlsx
@@ -970,18 +970,6 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1002,6 +990,18 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -1326,9 +1326,9 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:BW15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="BH1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="BN27" sqref="BN27"/>
+      <selection pane="bottomLeft" activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1787,7 +1787,7 @@
       <c r="A3" s="18" t="b">
         <v>0</v>
       </c>
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="47" t="s">
         <v>67</v>
       </c>
       <c r="C3" s="19"/>
@@ -1806,171 +1806,171 @@
       <c r="H3" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="I3" s="42" t="s">
+      <c r="I3" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="J3" s="42">
+      <c r="J3" s="38">
         <v>36</v>
       </c>
-      <c r="K3" s="42" t="s">
+      <c r="K3" s="38" t="s">
         <v>73</v>
       </c>
-      <c r="L3" s="45" t="s">
+      <c r="L3" s="41" t="s">
         <v>74</v>
       </c>
-      <c r="M3" s="45" t="s">
+      <c r="M3" s="41" t="s">
         <v>75</v>
       </c>
-      <c r="N3" s="42" t="s">
+      <c r="N3" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="O3" s="42" t="s">
+      <c r="O3" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="P3" s="42" t="s">
+      <c r="P3" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="Q3" s="42" t="s">
+      <c r="Q3" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="R3" s="42" t="s">
+      <c r="R3" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="S3" s="42" t="s">
+      <c r="S3" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="T3" s="42" t="s">
+      <c r="T3" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="U3" s="42" t="s">
+      <c r="U3" s="38" t="s">
         <v>83</v>
       </c>
-      <c r="V3" s="42">
+      <c r="V3" s="38">
         <v>323210</v>
       </c>
-      <c r="W3" s="45" t="s">
+      <c r="W3" s="41" t="s">
         <v>84</v>
       </c>
-      <c r="X3" s="42" t="s">
+      <c r="X3" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="Y3" s="42" t="s">
+      <c r="Y3" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="Z3" s="42" t="s">
+      <c r="Z3" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="AA3" s="42" t="s">
+      <c r="AA3" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="AB3" s="42" t="s">
+      <c r="AB3" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="AC3" s="42" t="s">
+      <c r="AC3" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="AD3" s="42" t="s">
+      <c r="AD3" s="38" t="s">
         <v>88</v>
       </c>
-      <c r="AE3" s="42" t="s">
+      <c r="AE3" s="38" t="s">
         <v>89</v>
       </c>
-      <c r="AF3" s="42" t="s">
+      <c r="AF3" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="AG3" s="42" t="s">
+      <c r="AG3" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="AH3" s="42" t="s">
+      <c r="AH3" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="AI3" s="42"/>
-      <c r="AJ3" s="42" t="s">
+      <c r="AI3" s="38"/>
+      <c r="AJ3" s="38" t="s">
         <v>92</v>
       </c>
-      <c r="AK3" s="42" t="s">
+      <c r="AK3" s="38" t="s">
         <v>93</v>
       </c>
-      <c r="AL3" s="42"/>
-      <c r="AM3" s="42" t="s">
+      <c r="AL3" s="38"/>
+      <c r="AM3" s="38" t="s">
         <v>94</v>
       </c>
-      <c r="AN3" s="42" t="s">
+      <c r="AN3" s="38" t="s">
         <v>95</v>
       </c>
-      <c r="AO3" s="42">
+      <c r="AO3" s="38">
         <v>123456789</v>
       </c>
-      <c r="AP3" s="42" t="s">
+      <c r="AP3" s="38" t="s">
         <v>96</v>
       </c>
-      <c r="AQ3" s="42"/>
-      <c r="AR3" s="42" t="s">
+      <c r="AQ3" s="38"/>
+      <c r="AR3" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="AS3" s="42">
+      <c r="AS3" s="38">
         <v>3305551234</v>
       </c>
-      <c r="AT3" s="42" t="s">
+      <c r="AT3" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="AU3" s="42" t="s">
+      <c r="AU3" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="AV3" s="42" t="s">
+      <c r="AV3" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="AW3" s="42" t="s">
+      <c r="AW3" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="AX3" s="42" t="s">
+      <c r="AX3" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="AY3" s="42" t="s">
+      <c r="AY3" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="AZ3" s="42" t="s">
+      <c r="AZ3" s="38" t="s">
         <v>98</v>
       </c>
-      <c r="BA3" s="42">
+      <c r="BA3" s="38">
         <v>1</v>
       </c>
-      <c r="BB3" s="42">
+      <c r="BB3" s="38">
         <v>250</v>
       </c>
-      <c r="BC3" s="42" t="s">
+      <c r="BC3" s="38" t="s">
         <v>92</v>
       </c>
-      <c r="BD3" s="42" t="s">
+      <c r="BD3" s="38" t="s">
         <v>73</v>
       </c>
-      <c r="BE3" s="42" t="s">
+      <c r="BE3" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="BF3" s="42" t="s">
+      <c r="BF3" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="BG3" s="42" t="s">
+      <c r="BG3" s="38" t="s">
         <v>101</v>
       </c>
-      <c r="BH3" s="42" t="s">
+      <c r="BH3" s="38" t="s">
         <v>100</v>
       </c>
       <c r="BI3" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="BJ3" s="42" t="s">
+      <c r="BJ3" s="38" t="s">
         <v>102</v>
       </c>
-      <c r="BK3" s="42" t="s">
+      <c r="BK3" s="38" t="s">
         <v>103</v>
       </c>
-      <c r="BL3" s="42"/>
-      <c r="BM3" s="42"/>
-      <c r="BN3" s="42" t="s">
+      <c r="BL3" s="38"/>
+      <c r="BM3" s="38"/>
+      <c r="BN3" s="38" t="s">
         <v>104</v>
       </c>
-      <c r="BO3" s="48" t="s">
+      <c r="BO3" s="44" t="s">
         <v>105</v>
       </c>
       <c r="BP3" s="22"/>
@@ -1986,7 +1986,7 @@
       <c r="A4" s="18" t="b">
         <v>0</v>
       </c>
-      <c r="B4" s="39"/>
+      <c r="B4" s="48"/>
       <c r="C4" s="23"/>
       <c r="D4" s="24" t="s">
         <v>106</v>
@@ -2155,7 +2155,7 @@
       <c r="A5" s="18" t="b">
         <v>0</v>
       </c>
-      <c r="B5" s="39"/>
+      <c r="B5" s="48"/>
       <c r="C5" s="23"/>
       <c r="D5" s="24" t="s">
         <v>114</v>
@@ -2324,7 +2324,7 @@
       <c r="A6" s="18" t="b">
         <v>0</v>
       </c>
-      <c r="B6" s="39"/>
+      <c r="B6" s="48"/>
       <c r="C6" s="23"/>
       <c r="D6" s="24" t="s">
         <v>114</v>
@@ -2493,7 +2493,7 @@
       <c r="A7" s="18" t="b">
         <v>0</v>
       </c>
-      <c r="B7" s="39"/>
+      <c r="B7" s="48"/>
       <c r="C7" s="23"/>
       <c r="D7" s="24" t="s">
         <v>114</v>
@@ -2662,7 +2662,7 @@
       <c r="A8" s="18" t="b">
         <v>0</v>
       </c>
-      <c r="B8" s="39"/>
+      <c r="B8" s="48"/>
       <c r="C8" s="23"/>
       <c r="D8" s="24" t="s">
         <v>114</v>
@@ -2831,7 +2831,7 @@
       <c r="A9" s="18" t="b">
         <v>0</v>
       </c>
-      <c r="B9" s="39"/>
+      <c r="B9" s="48"/>
       <c r="C9" s="23"/>
       <c r="D9" s="24" t="s">
         <v>122</v>
@@ -3000,7 +3000,7 @@
       <c r="A10" s="18" t="b">
         <v>0</v>
       </c>
-      <c r="B10" s="39"/>
+      <c r="B10" s="48"/>
       <c r="C10" s="23"/>
       <c r="D10" s="24" t="s">
         <v>114</v>
@@ -3171,7 +3171,7 @@
       <c r="A11" s="18" t="b">
         <v>0</v>
       </c>
-      <c r="B11" s="39"/>
+      <c r="B11" s="48"/>
       <c r="C11" s="23"/>
       <c r="D11" s="24" t="s">
         <v>130</v>
@@ -3340,7 +3340,7 @@
       <c r="A12" s="18" t="b">
         <v>0</v>
       </c>
-      <c r="B12" s="39"/>
+      <c r="B12" s="48"/>
       <c r="C12" s="23"/>
       <c r="D12" s="24" t="s">
         <v>122</v>
@@ -3360,16 +3360,16 @@
       <c r="I12" s="36" t="s">
         <v>72</v>
       </c>
-      <c r="J12" s="44">
+      <c r="J12" s="40">
         <v>20</v>
       </c>
       <c r="K12" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="L12" s="46" t="s">
+      <c r="L12" s="42" t="s">
         <v>74</v>
       </c>
-      <c r="M12" s="46" t="s">
+      <c r="M12" s="42" t="s">
         <v>75</v>
       </c>
       <c r="N12" s="36" t="s">
@@ -3399,7 +3399,7 @@
       <c r="V12" s="36">
         <v>323287</v>
       </c>
-      <c r="W12" s="46" t="s">
+      <c r="W12" s="42" t="s">
         <v>133</v>
       </c>
       <c r="X12" s="36" t="s">
@@ -3469,7 +3469,7 @@
       <c r="BD12" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="BE12" s="44">
+      <c r="BE12" s="40">
         <v>20</v>
       </c>
       <c r="BF12" s="36">
@@ -3495,7 +3495,7 @@
       <c r="BN12" s="36" t="s">
         <v>104</v>
       </c>
-      <c r="BO12" s="49" t="s">
+      <c r="BO12" s="45" t="s">
         <v>113</v>
       </c>
       <c r="BP12" s="22"/>
@@ -3511,7 +3511,7 @@
       <c r="A13" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="B13" s="40" t="s">
+      <c r="B13" s="49" t="s">
         <v>136</v>
       </c>
       <c r="C13" s="29" t="s">
@@ -3532,143 +3532,143 @@
       <c r="H13" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="I13" s="43" t="s">
+      <c r="I13" s="39" t="s">
         <v>72</v>
       </c>
-      <c r="J13" s="43">
+      <c r="J13" s="39">
         <v>105</v>
       </c>
-      <c r="K13" s="43" t="s">
+      <c r="K13" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="L13" s="47" t="s">
+      <c r="L13" s="43" t="s">
         <v>74</v>
       </c>
-      <c r="M13" s="47" t="s">
+      <c r="M13" s="43" t="s">
         <v>75</v>
       </c>
-      <c r="N13" s="43" t="s">
+      <c r="N13" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="O13" s="43" t="s">
+      <c r="O13" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="P13" s="43" t="s">
+      <c r="P13" s="39" t="s">
         <v>78</v>
       </c>
-      <c r="Q13" s="43" t="s">
+      <c r="Q13" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="R13" s="43" t="s">
+      <c r="R13" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="S13" s="43" t="s">
+      <c r="S13" s="39" t="s">
         <v>81</v>
       </c>
       <c r="T13" s="29"/>
-      <c r="U13" s="43" t="s">
+      <c r="U13" s="39" t="s">
         <v>83</v>
       </c>
-      <c r="V13" s="43" t="s">
+      <c r="V13" s="39" t="s">
         <v>137</v>
       </c>
-      <c r="W13" s="47" t="s">
+      <c r="W13" s="43" t="s">
         <v>139</v>
       </c>
-      <c r="X13" s="43" t="s">
+      <c r="X13" s="39" t="s">
         <v>140</v>
       </c>
-      <c r="Y13" s="43" t="s">
+      <c r="Y13" s="39" t="s">
         <v>141</v>
       </c>
-      <c r="Z13" s="43">
+      <c r="Z13" s="39">
         <v>30052</v>
       </c>
-      <c r="AA13" s="43" t="s">
+      <c r="AA13" s="39" t="s">
         <v>81</v>
       </c>
-      <c r="AB13" s="43" t="s">
+      <c r="AB13" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="AC13" s="43" t="b">
+      <c r="AC13" s="39" t="b">
         <v>0</v>
       </c>
-      <c r="AD13" s="43" t="s">
+      <c r="AD13" s="39" t="s">
         <v>88</v>
       </c>
-      <c r="AE13" s="43" t="s">
+      <c r="AE13" s="39" t="s">
         <v>89</v>
       </c>
-      <c r="AF13" s="43" t="s">
+      <c r="AF13" s="39" t="s">
         <v>90</v>
       </c>
-      <c r="AG13" s="43" t="s">
+      <c r="AG13" s="39" t="s">
         <v>81</v>
       </c>
-      <c r="AH13" s="43"/>
-      <c r="AI13" s="43"/>
-      <c r="AJ13" s="43"/>
-      <c r="AK13" s="43"/>
-      <c r="AL13" s="43"/>
-      <c r="AM13" s="43"/>
-      <c r="AN13" s="43"/>
-      <c r="AO13" s="43"/>
-      <c r="AP13" s="43"/>
-      <c r="AQ13" s="43"/>
-      <c r="AR13" s="43"/>
-      <c r="AS13" s="43"/>
-      <c r="AT13" s="43"/>
-      <c r="AU13" s="43"/>
-      <c r="AV13" s="43"/>
-      <c r="AW13" s="43"/>
-      <c r="AX13" s="43"/>
-      <c r="AY13" s="43"/>
-      <c r="AZ13" s="43" t="s">
+      <c r="AH13" s="39"/>
+      <c r="AI13" s="39"/>
+      <c r="AJ13" s="39"/>
+      <c r="AK13" s="39"/>
+      <c r="AL13" s="39"/>
+      <c r="AM13" s="39"/>
+      <c r="AN13" s="39"/>
+      <c r="AO13" s="39"/>
+      <c r="AP13" s="39"/>
+      <c r="AQ13" s="39"/>
+      <c r="AR13" s="39"/>
+      <c r="AS13" s="39"/>
+      <c r="AT13" s="39"/>
+      <c r="AU13" s="39"/>
+      <c r="AV13" s="39"/>
+      <c r="AW13" s="39"/>
+      <c r="AX13" s="39"/>
+      <c r="AY13" s="39"/>
+      <c r="AZ13" s="39" t="s">
         <v>98</v>
       </c>
-      <c r="BA13" s="43">
+      <c r="BA13" s="39">
         <v>1</v>
       </c>
-      <c r="BB13" s="43">
+      <c r="BB13" s="39">
         <v>250</v>
       </c>
-      <c r="BC13" s="43" t="s">
+      <c r="BC13" s="39" t="s">
         <v>92</v>
       </c>
-      <c r="BD13" s="43" t="s">
+      <c r="BD13" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="BE13" s="43">
+      <c r="BE13" s="39">
         <v>105</v>
       </c>
-      <c r="BF13" s="43">
+      <c r="BF13" s="39">
         <v>20</v>
       </c>
-      <c r="BG13" s="43">
+      <c r="BG13" s="39">
         <v>15</v>
       </c>
-      <c r="BH13" s="43">
+      <c r="BH13" s="39">
         <v>20</v>
       </c>
-      <c r="BI13" s="43" t="s">
+      <c r="BI13" s="39" t="s">
         <v>112</v>
       </c>
-      <c r="BJ13" s="43" t="s">
+      <c r="BJ13" s="39" t="s">
         <v>102</v>
       </c>
-      <c r="BK13" s="43" t="s">
+      <c r="BK13" s="39" t="s">
         <v>103</v>
       </c>
-      <c r="BL13" s="43" t="s">
+      <c r="BL13" s="39" t="s">
         <v>142</v>
       </c>
-      <c r="BM13" s="43" t="s">
+      <c r="BM13" s="39" t="s">
         <v>143</v>
       </c>
-      <c r="BN13" s="43" t="s">
+      <c r="BN13" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="BO13" s="50" t="s">
+      <c r="BO13" s="46" t="s">
         <v>113</v>
       </c>
       <c r="BP13" s="22"/>
@@ -3684,7 +3684,7 @@
       <c r="A14" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="B14" s="40"/>
+      <c r="B14" s="49"/>
       <c r="C14" s="29" t="s">
         <v>144</v>
       </c>
@@ -3706,11 +3706,11 @@
       <c r="I14" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="J14" s="29" t="s">
+      <c r="J14" s="29">
+        <v>500</v>
+      </c>
+      <c r="K14" s="29" t="s">
         <v>73</v>
-      </c>
-      <c r="K14" s="29">
-        <v>500</v>
       </c>
       <c r="L14" s="31" t="s">
         <v>74</v>
@@ -3855,7 +3855,7 @@
       <c r="A15" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="B15" s="41"/>
+      <c r="B15" s="50"/>
       <c r="C15" s="33" t="s">
         <v>153</v>
       </c>

</xml_diff>

<commit_message>
Add AlcoholRecipientType to FedExPrototypeFixture
</commit_message>
<xml_diff>
--- a/Code/ShipWorks.Tests.Integration/DataSources/FedExAll/US Exp Dom-Alcohol.xlsx
+++ b/Code/ShipWorks.Tests.Integration/DataSources/FedExAll/US Exp Dom-Alcohol.xlsx
@@ -120,391 +120,391 @@
     <t>RequestedPackageLineItems.SpecialServicesRequested.SpecialServiceTypes</t>
   </si>
   <si>
+    <t>TC #</t>
+  </si>
+  <si>
+    <t>CustomerTransactionId</t>
+  </si>
+  <si>
+    <t>DropoffType</t>
+  </si>
+  <si>
+    <t>ServiceType</t>
+  </si>
+  <si>
+    <t>PackagingType</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Units</t>
+  </si>
+  <si>
+    <t>PersonName</t>
+  </si>
+  <si>
+    <t>CompanyName</t>
+  </si>
+  <si>
+    <t>PhoneNumber</t>
+  </si>
+  <si>
+    <t>StreetLines</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>StateOrProvinceCode</t>
+  </si>
+  <si>
+    <t>PostalCode</t>
+  </si>
+  <si>
+    <t>CountryCode</t>
+  </si>
+  <si>
+    <t>Residential</t>
+  </si>
+  <si>
+    <t>PaymentType</t>
+  </si>
+  <si>
+    <t>AccountNumber</t>
+  </si>
+  <si>
+    <t>SpecialServiceTypes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SpecialServiceTypes </t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>AddTransportationCharges</t>
+  </si>
+  <si>
+    <t>CollectionType</t>
+  </si>
+  <si>
+    <t>TinType</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>ReferenceIndicator</t>
+  </si>
+  <si>
+    <t>RateRequestTypes</t>
+  </si>
+  <si>
+    <t>PackageCount</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>Width</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>CustomerReferenceType</t>
+  </si>
+  <si>
+    <t>SignatureOptionDetail</t>
+  </si>
+  <si>
+    <t>RecipientType</t>
+  </si>
+  <si>
+    <t>REVENUE</t>
+  </si>
+  <si>
+    <t>Alcohol, COD, Your Packaging, Express Saver</t>
+  </si>
+  <si>
+    <t>FDXShipRequest</t>
+  </si>
+  <si>
+    <t>REGULAR_PICKUP</t>
+  </si>
+  <si>
+    <t>FEDEX_EXPRESS_SAVER</t>
+  </si>
+  <si>
+    <t>YOUR_PACKAGING</t>
+  </si>
+  <si>
+    <t>LB</t>
+  </si>
+  <si>
+    <t>James Weston</t>
+  </si>
+  <si>
+    <t>RTC</t>
+  </si>
+  <si>
+    <t>9012633035</t>
+  </si>
+  <si>
+    <t>1751 THOMPSON ST</t>
+  </si>
+  <si>
+    <t>AURORA</t>
+  </si>
+  <si>
+    <t>OH</t>
+  </si>
+  <si>
+    <t>44202</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>CSP testing</t>
+  </si>
+  <si>
+    <t>110 Fedex parkway</t>
+  </si>
+  <si>
+    <t>NEW ORLEANS</t>
+  </si>
+  <si>
+    <t>LA</t>
+  </si>
+  <si>
+    <t>70119</t>
+  </si>
+  <si>
+    <t>SENDER</t>
+  </si>
+  <si>
+    <t>Please use shipper account number</t>
+  </si>
+  <si>
+    <t>CSP Testing</t>
+  </si>
+  <si>
+    <t>COD Each Package</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>100 Each Package</t>
+  </si>
+  <si>
+    <t>ANY Each Package</t>
+  </si>
+  <si>
+    <t>PERSONAL_STATE</t>
+  </si>
+  <si>
+    <t>CSP</t>
+  </si>
+  <si>
+    <t>INVOICE</t>
+  </si>
+  <si>
+    <t>LIST</t>
+  </si>
+  <si>
+    <t>18 Each Package</t>
+  </si>
+  <si>
+    <t>20 Each Package</t>
+  </si>
+  <si>
+    <t>15 Each Package</t>
+  </si>
+  <si>
+    <t>CUSTOMER_REFERENCE</t>
+  </si>
+  <si>
+    <t>$AW</t>
+  </si>
+  <si>
+    <t>ALCOHOL</t>
+  </si>
+  <si>
+    <t>CONSUMER</t>
+  </si>
+  <si>
+    <t>Alcohol, Your Packaging, 2 day</t>
+  </si>
+  <si>
+    <t>FEDEX_2_DAY</t>
+  </si>
+  <si>
+    <t>86 Fedex parkway</t>
+  </si>
+  <si>
+    <t>PADUCAH</t>
+  </si>
+  <si>
+    <t>KY</t>
+  </si>
+  <si>
+    <t>42001</t>
+  </si>
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>LICENSEE</t>
+  </si>
+  <si>
+    <t>Alcohol, Your Packaging, Priority Overnight</t>
+  </si>
+  <si>
+    <t>PRIORITY_OVERNIGHT</t>
+  </si>
+  <si>
+    <t>9 Fedex parkway</t>
+  </si>
+  <si>
+    <t>9.0</t>
+  </si>
+  <si>
+    <t>126 Fedex parkway</t>
+  </si>
+  <si>
+    <t>RECIPIENT</t>
+  </si>
+  <si>
+    <t>134 Fedex parkway</t>
+  </si>
+  <si>
+    <t>144 Fedex parkway</t>
+  </si>
+  <si>
+    <t>Alcohol, Your Packaging, First Overnight</t>
+  </si>
+  <si>
+    <t>REQUEST_COURIER</t>
+  </si>
+  <si>
+    <t>FIRST_OVERNIGHT</t>
+  </si>
+  <si>
+    <t>17 Fedex parkway</t>
+  </si>
+  <si>
+    <t>42 Fedex parkway</t>
+  </si>
+  <si>
+    <t>ANCHORAGE</t>
+  </si>
+  <si>
+    <t>AK</t>
+  </si>
+  <si>
+    <t>99501</t>
+  </si>
+  <si>
+    <t>Alcohol, Your Packaging, Standard Overnight</t>
+  </si>
+  <si>
+    <t>STANDARD_OVERNIGHT</t>
+  </si>
+  <si>
+    <t>58 Fedex parkway</t>
+  </si>
+  <si>
+    <t>20 Fedex parkway</t>
+  </si>
+  <si>
+    <t>FEDERAL WAY</t>
+  </si>
+  <si>
+    <t>WA</t>
+  </si>
+  <si>
+    <t>REVENUE + LABELS</t>
+  </si>
+  <si>
+    <t>PO7</t>
+  </si>
+  <si>
+    <t>Alcohol, Priority Overnight Cust Pkg</t>
+  </si>
+  <si>
+    <t>20 FedEx Pkwy</t>
+  </si>
+  <si>
+    <t>Loganville</t>
+  </si>
+  <si>
+    <t>GA</t>
+  </si>
+  <si>
+    <t>SIGNATURE_OPTION</t>
+  </si>
+  <si>
+    <t>ADULT</t>
+  </si>
+  <si>
+    <t>EF1</t>
+  </si>
+  <si>
+    <t>Alcohol, Your Packaging, 1day freight,Sat Pickup,Adult signature</t>
+  </si>
+  <si>
+    <t>FEDEX_1_DAY_FREIGHT</t>
+  </si>
+  <si>
+    <t>128 Fedex parkway</t>
+  </si>
+  <si>
+    <t>Gowrie</t>
+  </si>
+  <si>
+    <t>IA</t>
+  </si>
+  <si>
+    <t>50543</t>
+  </si>
+  <si>
+    <t>RTC Testing</t>
+  </si>
+  <si>
+    <t>SATURDAY_PICKUP</t>
+  </si>
+  <si>
+    <t>ES4</t>
+  </si>
+  <si>
+    <t>Alcohol, 2day, Cust Pkg</t>
+  </si>
+  <si>
+    <t>Spokane</t>
+  </si>
+  <si>
+    <t>COD</t>
+  </si>
+  <si>
+    <t>GUARANTEED_FUNDS</t>
+  </si>
+  <si>
+    <t>DIRECT</t>
+  </si>
+  <si>
     <t>RequestedPackageLineItems.SpecialServicesRequested.SpecialServiceTypes.AlcoholDetail</t>
-  </si>
-  <si>
-    <t>TC #</t>
-  </si>
-  <si>
-    <t>CustomerTransactionId</t>
-  </si>
-  <si>
-    <t>DropoffType</t>
-  </si>
-  <si>
-    <t>ServiceType</t>
-  </si>
-  <si>
-    <t>PackagingType</t>
-  </si>
-  <si>
-    <t>Value</t>
-  </si>
-  <si>
-    <t>Units</t>
-  </si>
-  <si>
-    <t>PersonName</t>
-  </si>
-  <si>
-    <t>CompanyName</t>
-  </si>
-  <si>
-    <t>PhoneNumber</t>
-  </si>
-  <si>
-    <t>StreetLines</t>
-  </si>
-  <si>
-    <t>City</t>
-  </si>
-  <si>
-    <t>StateOrProvinceCode</t>
-  </si>
-  <si>
-    <t>PostalCode</t>
-  </si>
-  <si>
-    <t>CountryCode</t>
-  </si>
-  <si>
-    <t>Residential</t>
-  </si>
-  <si>
-    <t>PaymentType</t>
-  </si>
-  <si>
-    <t>AccountNumber</t>
-  </si>
-  <si>
-    <t>SpecialServiceTypes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SpecialServiceTypes </t>
-  </si>
-  <si>
-    <t>Currency</t>
-  </si>
-  <si>
-    <t>Amount</t>
-  </si>
-  <si>
-    <t>AddTransportationCharges</t>
-  </si>
-  <si>
-    <t>CollectionType</t>
-  </si>
-  <si>
-    <t>TinType</t>
-  </si>
-  <si>
-    <t>Number</t>
-  </si>
-  <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t>ReferenceIndicator</t>
-  </si>
-  <si>
-    <t>RateRequestTypes</t>
-  </si>
-  <si>
-    <t>PackageCount</t>
-  </si>
-  <si>
-    <t>Length</t>
-  </si>
-  <si>
-    <t>Width</t>
-  </si>
-  <si>
-    <t>Height</t>
-  </si>
-  <si>
-    <t>CustomerReferenceType</t>
-  </si>
-  <si>
-    <t>SignatureOptionDetail</t>
-  </si>
-  <si>
-    <t>RecipientType</t>
-  </si>
-  <si>
-    <t>REVENUE</t>
-  </si>
-  <si>
-    <t>Alcohol, COD, Your Packaging, Express Saver</t>
-  </si>
-  <si>
-    <t>FDXShipRequest</t>
-  </si>
-  <si>
-    <t>REGULAR_PICKUP</t>
-  </si>
-  <si>
-    <t>FEDEX_EXPRESS_SAVER</t>
-  </si>
-  <si>
-    <t>YOUR_PACKAGING</t>
-  </si>
-  <si>
-    <t>LB</t>
-  </si>
-  <si>
-    <t>James Weston</t>
-  </si>
-  <si>
-    <t>RTC</t>
-  </si>
-  <si>
-    <t>9012633035</t>
-  </si>
-  <si>
-    <t>1751 THOMPSON ST</t>
-  </si>
-  <si>
-    <t>AURORA</t>
-  </si>
-  <si>
-    <t>OH</t>
-  </si>
-  <si>
-    <t>44202</t>
-  </si>
-  <si>
-    <t>US</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>CSP testing</t>
-  </si>
-  <si>
-    <t>110 Fedex parkway</t>
-  </si>
-  <si>
-    <t>NEW ORLEANS</t>
-  </si>
-  <si>
-    <t>LA</t>
-  </si>
-  <si>
-    <t>70119</t>
-  </si>
-  <si>
-    <t>SENDER</t>
-  </si>
-  <si>
-    <t>Please use shipper account number</t>
-  </si>
-  <si>
-    <t>CSP Testing</t>
-  </si>
-  <si>
-    <t>COD Each Package</t>
-  </si>
-  <si>
-    <t>USD</t>
-  </si>
-  <si>
-    <t>100 Each Package</t>
-  </si>
-  <si>
-    <t>ANY Each Package</t>
-  </si>
-  <si>
-    <t>PERSONAL_STATE</t>
-  </si>
-  <si>
-    <t>CSP</t>
-  </si>
-  <si>
-    <t>INVOICE</t>
-  </si>
-  <si>
-    <t>LIST</t>
-  </si>
-  <si>
-    <t>18 Each Package</t>
-  </si>
-  <si>
-    <t>20 Each Package</t>
-  </si>
-  <si>
-    <t>15 Each Package</t>
-  </si>
-  <si>
-    <t>CUSTOMER_REFERENCE</t>
-  </si>
-  <si>
-    <t>$AW</t>
-  </si>
-  <si>
-    <t>ALCOHOL</t>
-  </si>
-  <si>
-    <t>CONSUMER</t>
-  </si>
-  <si>
-    <t>Alcohol, Your Packaging, 2 day</t>
-  </si>
-  <si>
-    <t>FEDEX_2_DAY</t>
-  </si>
-  <si>
-    <t>86 Fedex parkway</t>
-  </si>
-  <si>
-    <t>PADUCAH</t>
-  </si>
-  <si>
-    <t>KY</t>
-  </si>
-  <si>
-    <t>42001</t>
-  </si>
-  <si>
-    <t>IN</t>
-  </si>
-  <si>
-    <t>LICENSEE</t>
-  </si>
-  <si>
-    <t>Alcohol, Your Packaging, Priority Overnight</t>
-  </si>
-  <si>
-    <t>PRIORITY_OVERNIGHT</t>
-  </si>
-  <si>
-    <t>9 Fedex parkway</t>
-  </si>
-  <si>
-    <t>9.0</t>
-  </si>
-  <si>
-    <t>126 Fedex parkway</t>
-  </si>
-  <si>
-    <t>RECIPIENT</t>
-  </si>
-  <si>
-    <t>134 Fedex parkway</t>
-  </si>
-  <si>
-    <t>144 Fedex parkway</t>
-  </si>
-  <si>
-    <t>Alcohol, Your Packaging, First Overnight</t>
-  </si>
-  <si>
-    <t>REQUEST_COURIER</t>
-  </si>
-  <si>
-    <t>FIRST_OVERNIGHT</t>
-  </si>
-  <si>
-    <t>17 Fedex parkway</t>
-  </si>
-  <si>
-    <t>42 Fedex parkway</t>
-  </si>
-  <si>
-    <t>ANCHORAGE</t>
-  </si>
-  <si>
-    <t>AK</t>
-  </si>
-  <si>
-    <t>99501</t>
-  </si>
-  <si>
-    <t>Alcohol, Your Packaging, Standard Overnight</t>
-  </si>
-  <si>
-    <t>STANDARD_OVERNIGHT</t>
-  </si>
-  <si>
-    <t>58 Fedex parkway</t>
-  </si>
-  <si>
-    <t>20 Fedex parkway</t>
-  </si>
-  <si>
-    <t>FEDERAL WAY</t>
-  </si>
-  <si>
-    <t>WA</t>
-  </si>
-  <si>
-    <t>REVENUE + LABELS</t>
-  </si>
-  <si>
-    <t>PO7</t>
-  </si>
-  <si>
-    <t>Alcohol, Priority Overnight Cust Pkg</t>
-  </si>
-  <si>
-    <t>20 FedEx Pkwy</t>
-  </si>
-  <si>
-    <t>Loganville</t>
-  </si>
-  <si>
-    <t>GA</t>
-  </si>
-  <si>
-    <t>SIGNATURE_OPTION</t>
-  </si>
-  <si>
-    <t>ADULT</t>
-  </si>
-  <si>
-    <t>EF1</t>
-  </si>
-  <si>
-    <t>Alcohol, Your Packaging, 1day freight,Sat Pickup,Adult signature</t>
-  </si>
-  <si>
-    <t>FEDEX_1_DAY_FREIGHT</t>
-  </si>
-  <si>
-    <t>128 Fedex parkway</t>
-  </si>
-  <si>
-    <t>Gowrie</t>
-  </si>
-  <si>
-    <t>IA</t>
-  </si>
-  <si>
-    <t>50543</t>
-  </si>
-  <si>
-    <t>RTC Testing</t>
-  </si>
-  <si>
-    <t>SATURDAY_PICKUP</t>
-  </si>
-  <si>
-    <t>ES4</t>
-  </si>
-  <si>
-    <t>Alcohol, 2day, Cust Pkg</t>
-  </si>
-  <si>
-    <t>Spokane</t>
-  </si>
-  <si>
-    <t>COD</t>
-  </si>
-  <si>
-    <t>GUARANTEED_FUNDS</t>
-  </si>
-  <si>
-    <t>DIRECT</t>
   </si>
 </sst>
 </file>
@@ -1326,9 +1326,9 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:BW15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="BG1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K27" sqref="K27"/>
+      <selection pane="bottomLeft" activeCell="BO1" sqref="BO1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1588,199 +1588,199 @@
         <v>28</v>
       </c>
       <c r="BO1" s="7" t="s">
-        <v>30</v>
+        <v>158</v>
       </c>
     </row>
     <row r="2" spans="1:75" s="9" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="10"/>
       <c r="C2" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D2" s="12"/>
       <c r="E2" s="12"/>
       <c r="F2" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="H2" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="I2" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="J2" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="K2" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="L2" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="L2" s="12" t="s">
+      <c r="M2" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="M2" s="12" t="s">
+      <c r="N2" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="N2" s="12" t="s">
+      <c r="O2" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="O2" s="12" t="s">
+      <c r="P2" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="P2" s="12" t="s">
+      <c r="Q2" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="Q2" s="12" t="s">
+      <c r="R2" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="R2" s="12" t="s">
+      <c r="S2" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="S2" s="12" t="s">
+      <c r="T2" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="T2" s="12" t="s">
+      <c r="U2" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="V2" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="W2" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="X2" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y2" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z2" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA2" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB2" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC2" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="AD2" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="U2" s="12" t="s">
+      <c r="AE2" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="AF2" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="AG2" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="AH2" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="AI2" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="AJ2" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="AK2" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="AL2" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="AM2" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="AN2" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO2" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="AP2" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="AQ2" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="AR2" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="AS2" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="V2" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="W2" s="12" t="s">
+      <c r="AT2" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="AU2" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="X2" s="12" t="s">
+      <c r="AV2" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="Y2" s="12" t="s">
+      <c r="AW2" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="Z2" s="12" t="s">
+      <c r="AX2" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="AA2" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="AB2" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC2" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="AD2" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="AE2" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="AF2" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="AG2" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="AH2" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="AI2" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="AJ2" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="AK2" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="AL2" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="AM2" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="AN2" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="AO2" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="AP2" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="AQ2" s="12" t="s">
+      <c r="AY2" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="AR2" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="AS2" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="AT2" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="AU2" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="AV2" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="AW2" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="AX2" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="AY2" s="12" t="s">
+      <c r="AZ2" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="AZ2" s="16" t="s">
+      <c r="BA2" s="12" t="s">
         <v>59</v>
-      </c>
-      <c r="BA2" s="12" t="s">
-        <v>60</v>
       </c>
       <c r="BB2" s="12"/>
       <c r="BC2" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="BD2" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="BE2" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="BF2" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="BG2" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="BH2" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="BI2" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="BF2" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="BG2" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="BH2" s="12" t="s">
+      <c r="BJ2" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="BI2" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="BJ2" s="12" t="s">
+      <c r="BK2" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="BL2" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="BM2" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="BK2" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="BL2" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="BM2" s="17" t="s">
+      <c r="BN2" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="BO2" s="16" t="s">
         <v>65</v>
-      </c>
-      <c r="BN2" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="BO2" s="16" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:75" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1788,149 +1788,149 @@
         <v>0</v>
       </c>
       <c r="B3" s="47" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C3" s="19"/>
       <c r="D3" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="21" t="s">
         <v>68</v>
-      </c>
-      <c r="E3" s="21" t="s">
-        <v>69</v>
       </c>
       <c r="F3" s="19">
         <v>323210</v>
       </c>
       <c r="G3" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="H3" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="H3" s="19" t="s">
+      <c r="I3" s="38" t="s">
         <v>71</v>
-      </c>
-      <c r="I3" s="38" t="s">
-        <v>72</v>
       </c>
       <c r="J3" s="38">
         <v>36</v>
       </c>
       <c r="K3" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="L3" s="41" t="s">
         <v>73</v>
       </c>
-      <c r="L3" s="41" t="s">
+      <c r="M3" s="41" t="s">
         <v>74</v>
       </c>
-      <c r="M3" s="41" t="s">
+      <c r="N3" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="N3" s="38" t="s">
+      <c r="O3" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="O3" s="38" t="s">
+      <c r="P3" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="P3" s="38" t="s">
+      <c r="Q3" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="Q3" s="38" t="s">
+      <c r="R3" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="R3" s="38" t="s">
+      <c r="S3" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="S3" s="38" t="s">
+      <c r="T3" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="T3" s="38" t="s">
+      <c r="U3" s="38" t="s">
         <v>82</v>
-      </c>
-      <c r="U3" s="38" t="s">
-        <v>83</v>
       </c>
       <c r="V3" s="38">
         <v>323210</v>
       </c>
       <c r="W3" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="X3" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="X3" s="38" t="s">
+      <c r="Y3" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="Y3" s="38" t="s">
+      <c r="Z3" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="Z3" s="38" t="s">
+      <c r="AA3" s="38" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB3" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC3" s="38" t="s">
+        <v>81</v>
+      </c>
+      <c r="AD3" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="AA3" s="38" t="s">
-        <v>81</v>
-      </c>
-      <c r="AB3" s="38" t="s">
-        <v>76</v>
-      </c>
-      <c r="AC3" s="38" t="s">
-        <v>82</v>
-      </c>
-      <c r="AD3" s="38" t="s">
+      <c r="AE3" s="38" t="s">
         <v>88</v>
       </c>
-      <c r="AE3" s="38" t="s">
+      <c r="AF3" s="38" t="s">
         <v>89</v>
       </c>
-      <c r="AF3" s="38" t="s">
+      <c r="AG3" s="38" t="s">
+        <v>80</v>
+      </c>
+      <c r="AH3" s="38" t="s">
         <v>90</v>
-      </c>
-      <c r="AG3" s="38" t="s">
-        <v>81</v>
-      </c>
-      <c r="AH3" s="38" t="s">
-        <v>91</v>
       </c>
       <c r="AI3" s="38"/>
       <c r="AJ3" s="38" t="s">
+        <v>91</v>
+      </c>
+      <c r="AK3" s="38" t="s">
         <v>92</v>
-      </c>
-      <c r="AK3" s="38" t="s">
-        <v>93</v>
       </c>
       <c r="AL3" s="38"/>
       <c r="AM3" s="38" t="s">
+        <v>93</v>
+      </c>
+      <c r="AN3" s="38" t="s">
         <v>94</v>
-      </c>
-      <c r="AN3" s="38" t="s">
-        <v>95</v>
       </c>
       <c r="AO3" s="38">
         <v>123456789</v>
       </c>
       <c r="AP3" s="38" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AQ3" s="38"/>
       <c r="AR3" s="38" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AS3" s="38">
         <v>3305551234</v>
       </c>
       <c r="AT3" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="AU3" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="AU3" s="38" t="s">
+      <c r="AV3" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="AV3" s="38" t="s">
+      <c r="AW3" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="AW3" s="38" t="s">
+      <c r="AX3" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="AX3" s="38" t="s">
-        <v>81</v>
-      </c>
       <c r="AY3" s="38" t="s">
+        <v>96</v>
+      </c>
+      <c r="AZ3" s="38" t="s">
         <v>97</v>
-      </c>
-      <c r="AZ3" s="38" t="s">
-        <v>98</v>
       </c>
       <c r="BA3" s="38">
         <v>1</v>
@@ -1939,39 +1939,39 @@
         <v>250</v>
       </c>
       <c r="BC3" s="38" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="BD3" s="38" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="BE3" s="38" t="s">
+        <v>98</v>
+      </c>
+      <c r="BF3" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="BF3" s="38" t="s">
+      <c r="BG3" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="BG3" s="38" t="s">
+      <c r="BH3" s="38" t="s">
+        <v>99</v>
+      </c>
+      <c r="BI3" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="BJ3" s="38" t="s">
         <v>101</v>
       </c>
-      <c r="BH3" s="38" t="s">
-        <v>100</v>
-      </c>
-      <c r="BI3" s="23" t="s">
-        <v>112</v>
-      </c>
-      <c r="BJ3" s="38" t="s">
+      <c r="BK3" s="38" t="s">
         <v>102</v>
-      </c>
-      <c r="BK3" s="38" t="s">
-        <v>103</v>
       </c>
       <c r="BL3" s="38"/>
       <c r="BM3" s="38"/>
       <c r="BN3" s="38" t="s">
+        <v>103</v>
+      </c>
+      <c r="BO3" s="44" t="s">
         <v>104</v>
-      </c>
-      <c r="BO3" s="44" t="s">
-        <v>105</v>
       </c>
       <c r="BP3" s="22"/>
       <c r="BQ3" s="22"/>
@@ -1989,100 +1989,100 @@
       <c r="B4" s="48"/>
       <c r="C4" s="23"/>
       <c r="D4" s="24" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E4" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F4" s="23">
         <v>323217</v>
       </c>
       <c r="G4" s="23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H4" s="23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I4" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J4" s="23">
         <v>9</v>
       </c>
       <c r="K4" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="L4" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="L4" s="25" t="s">
+      <c r="M4" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="M4" s="25" t="s">
+      <c r="N4" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="N4" s="23" t="s">
+      <c r="O4" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="O4" s="23" t="s">
+      <c r="P4" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="P4" s="23" t="s">
+      <c r="Q4" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="Q4" s="23" t="s">
+      <c r="R4" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="R4" s="23" t="s">
+      <c r="S4" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="S4" s="23" t="s">
+      <c r="T4" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="T4" s="23" t="s">
+      <c r="U4" s="23" t="s">
         <v>82</v>
-      </c>
-      <c r="U4" s="23" t="s">
-        <v>83</v>
       </c>
       <c r="V4" s="23">
         <v>323217</v>
       </c>
       <c r="W4" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="X4" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="X4" s="23" t="s">
+      <c r="Y4" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="Y4" s="23" t="s">
+      <c r="Z4" s="23" t="s">
         <v>110</v>
       </c>
-      <c r="Z4" s="23" t="s">
-        <v>111</v>
-      </c>
       <c r="AA4" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB4" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC4" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="AB4" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="AC4" s="23" t="s">
-        <v>82</v>
-      </c>
       <c r="AD4" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE4" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="AE4" s="23" t="s">
+      <c r="AF4" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="AF4" s="23" t="s">
-        <v>90</v>
-      </c>
       <c r="AG4" s="23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AH4" s="23"/>
       <c r="AI4" s="23"/>
       <c r="AJ4" s="23"/>
       <c r="AK4" s="23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AL4" s="23"/>
       <c r="AM4" s="23"/>
@@ -2099,7 +2099,7 @@
       <c r="AX4" s="23"/>
       <c r="AY4" s="23"/>
       <c r="AZ4" s="23" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="BA4" s="23">
         <v>1</v>
@@ -2108,10 +2108,10 @@
         <v>250</v>
       </c>
       <c r="BC4" s="23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="BD4" s="23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="BE4" s="23">
         <v>9</v>
@@ -2126,21 +2126,21 @@
         <v>20</v>
       </c>
       <c r="BI4" s="23" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="BJ4" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="BK4" s="23" t="s">
         <v>102</v>
-      </c>
-      <c r="BK4" s="23" t="s">
-        <v>103</v>
       </c>
       <c r="BL4" s="23"/>
       <c r="BM4" s="23"/>
       <c r="BN4" s="23" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="BO4" s="26" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="BP4" s="22"/>
       <c r="BQ4" s="22"/>
@@ -2158,100 +2158,100 @@
       <c r="B5" s="48"/>
       <c r="C5" s="23"/>
       <c r="D5" s="24" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E5" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F5" s="23">
         <v>323238</v>
       </c>
       <c r="G5" s="23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H5" s="23" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I5" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J5" s="23">
         <v>9</v>
       </c>
       <c r="K5" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="L5" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="L5" s="25" t="s">
+      <c r="M5" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="M5" s="25" t="s">
+      <c r="N5" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="N5" s="23" t="s">
+      <c r="O5" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="O5" s="23" t="s">
+      <c r="P5" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="P5" s="23" t="s">
+      <c r="Q5" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="Q5" s="23" t="s">
+      <c r="R5" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="R5" s="23" t="s">
+      <c r="S5" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="S5" s="23" t="s">
+      <c r="T5" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="T5" s="23" t="s">
+      <c r="U5" s="23" t="s">
         <v>82</v>
-      </c>
-      <c r="U5" s="23" t="s">
-        <v>83</v>
       </c>
       <c r="V5" s="23">
         <v>323238</v>
       </c>
       <c r="W5" s="25" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="X5" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="Y5" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="Y5" s="23" t="s">
+      <c r="Z5" s="23" t="s">
         <v>110</v>
       </c>
-      <c r="Z5" s="23" t="s">
-        <v>111</v>
-      </c>
       <c r="AA5" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB5" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC5" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="AB5" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="AC5" s="23" t="s">
-        <v>82</v>
-      </c>
       <c r="AD5" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE5" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="AE5" s="23" t="s">
+      <c r="AF5" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="AF5" s="23" t="s">
-        <v>90</v>
-      </c>
       <c r="AG5" s="23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AH5" s="23"/>
       <c r="AI5" s="23"/>
       <c r="AJ5" s="23"/>
       <c r="AK5" s="23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AL5" s="23"/>
       <c r="AM5" s="23"/>
@@ -2268,7 +2268,7 @@
       <c r="AX5" s="23"/>
       <c r="AY5" s="23"/>
       <c r="AZ5" s="23" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="BA5" s="23">
         <v>1</v>
@@ -2277,10 +2277,10 @@
         <v>250</v>
       </c>
       <c r="BC5" s="23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="BD5" s="23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="BE5" s="23">
         <v>9</v>
@@ -2295,21 +2295,21 @@
         <v>20</v>
       </c>
       <c r="BI5" s="23" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="BJ5" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="BK5" s="23" t="s">
         <v>102</v>
-      </c>
-      <c r="BK5" s="23" t="s">
-        <v>103</v>
       </c>
       <c r="BL5" s="23"/>
       <c r="BM5" s="23"/>
       <c r="BN5" s="23" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="BO5" s="26" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="BP5" s="22"/>
       <c r="BQ5" s="22"/>
@@ -2327,100 +2327,100 @@
       <c r="B6" s="48"/>
       <c r="C6" s="23"/>
       <c r="D6" s="24" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E6" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F6" s="23">
         <v>323259</v>
       </c>
       <c r="G6" s="23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H6" s="23" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I6" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="J6" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="K6" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="J6" s="27" t="s">
-        <v>117</v>
-      </c>
-      <c r="K6" s="23" t="s">
+      <c r="L6" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="L6" s="25" t="s">
+      <c r="M6" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="M6" s="25" t="s">
+      <c r="N6" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="N6" s="23" t="s">
+      <c r="O6" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="O6" s="23" t="s">
+      <c r="P6" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="P6" s="23" t="s">
+      <c r="Q6" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="Q6" s="23" t="s">
+      <c r="R6" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="R6" s="23" t="s">
+      <c r="S6" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="S6" s="23" t="s">
+      <c r="T6" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="T6" s="23" t="s">
+      <c r="U6" s="23" t="s">
         <v>82</v>
-      </c>
-      <c r="U6" s="23" t="s">
-        <v>83</v>
       </c>
       <c r="V6" s="23">
         <v>323259</v>
       </c>
       <c r="W6" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="X6" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y6" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z6" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="AA6" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB6" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC6" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="AD6" s="23" t="s">
         <v>118</v>
-      </c>
-      <c r="X6" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="Y6" s="23" t="s">
-        <v>86</v>
-      </c>
-      <c r="Z6" s="23" t="s">
-        <v>87</v>
-      </c>
-      <c r="AA6" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="AB6" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="AC6" s="23" t="s">
-        <v>82</v>
-      </c>
-      <c r="AD6" s="23" t="s">
-        <v>119</v>
       </c>
       <c r="AE6" s="23">
         <v>150067600</v>
       </c>
       <c r="AF6" s="23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AG6" s="23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AH6" s="23"/>
       <c r="AI6" s="23"/>
       <c r="AJ6" s="23"/>
       <c r="AK6" s="23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AL6" s="23"/>
       <c r="AM6" s="23"/>
@@ -2437,7 +2437,7 @@
       <c r="AX6" s="23"/>
       <c r="AY6" s="23"/>
       <c r="AZ6" s="23" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="BA6" s="23">
         <v>1</v>
@@ -2446,13 +2446,13 @@
         <v>250</v>
       </c>
       <c r="BC6" s="23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="BD6" s="23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="BE6" s="27" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="BF6" s="23">
         <v>10</v>
@@ -2464,21 +2464,21 @@
         <v>10</v>
       </c>
       <c r="BI6" s="23" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="BJ6" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="BK6" s="23" t="s">
         <v>102</v>
-      </c>
-      <c r="BK6" s="23" t="s">
-        <v>103</v>
       </c>
       <c r="BL6" s="23"/>
       <c r="BM6" s="23"/>
       <c r="BN6" s="23" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="BO6" s="26" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="BP6" s="22"/>
       <c r="BQ6" s="22"/>
@@ -2496,100 +2496,100 @@
       <c r="B7" s="48"/>
       <c r="C7" s="23"/>
       <c r="D7" s="24" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E7" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F7" s="23">
         <v>323267</v>
       </c>
       <c r="G7" s="23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H7" s="23" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I7" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="J7" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="K7" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="J7" s="27" t="s">
-        <v>117</v>
-      </c>
-      <c r="K7" s="23" t="s">
+      <c r="L7" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="L7" s="25" t="s">
+      <c r="M7" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="M7" s="25" t="s">
+      <c r="N7" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="N7" s="23" t="s">
+      <c r="O7" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="O7" s="23" t="s">
+      <c r="P7" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="P7" s="23" t="s">
+      <c r="Q7" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="Q7" s="23" t="s">
+      <c r="R7" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="R7" s="23" t="s">
+      <c r="S7" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="S7" s="23" t="s">
+      <c r="T7" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="T7" s="23" t="s">
+      <c r="U7" s="23" t="s">
         <v>82</v>
-      </c>
-      <c r="U7" s="23" t="s">
-        <v>83</v>
       </c>
       <c r="V7" s="23">
         <v>323267</v>
       </c>
       <c r="W7" s="25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="X7" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y7" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="Y7" s="23" t="s">
+      <c r="Z7" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="Z7" s="23" t="s">
-        <v>87</v>
-      </c>
       <c r="AA7" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB7" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC7" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="AB7" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="AC7" s="23" t="s">
-        <v>82</v>
-      </c>
       <c r="AD7" s="23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AE7" s="23">
         <v>150067600</v>
       </c>
       <c r="AF7" s="23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AG7" s="23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AH7" s="23"/>
       <c r="AI7" s="23"/>
       <c r="AJ7" s="23"/>
       <c r="AK7" s="23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AL7" s="23"/>
       <c r="AM7" s="23"/>
@@ -2606,7 +2606,7 @@
       <c r="AX7" s="23"/>
       <c r="AY7" s="23"/>
       <c r="AZ7" s="23" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="BA7" s="23">
         <v>1</v>
@@ -2615,13 +2615,13 @@
         <v>250</v>
       </c>
       <c r="BC7" s="23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="BD7" s="23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="BE7" s="27" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="BF7" s="23">
         <v>10</v>
@@ -2633,21 +2633,21 @@
         <v>10</v>
       </c>
       <c r="BI7" s="23" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="BJ7" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="BK7" s="23" t="s">
         <v>102</v>
-      </c>
-      <c r="BK7" s="23" t="s">
-        <v>103</v>
       </c>
       <c r="BL7" s="23"/>
       <c r="BM7" s="23"/>
       <c r="BN7" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="BO7" s="26" t="s">
         <v>104</v>
-      </c>
-      <c r="BO7" s="26" t="s">
-        <v>105</v>
       </c>
       <c r="BP7" s="22"/>
       <c r="BQ7" s="22"/>
@@ -2665,100 +2665,100 @@
       <c r="B8" s="48"/>
       <c r="C8" s="23"/>
       <c r="D8" s="24" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E8" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F8" s="23">
         <v>323277</v>
       </c>
       <c r="G8" s="23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H8" s="23" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I8" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="J8" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="K8" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="J8" s="27" t="s">
-        <v>117</v>
-      </c>
-      <c r="K8" s="23" t="s">
+      <c r="L8" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="L8" s="25" t="s">
+      <c r="M8" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="M8" s="25" t="s">
+      <c r="N8" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="N8" s="23" t="s">
+      <c r="O8" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="O8" s="23" t="s">
+      <c r="P8" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="P8" s="23" t="s">
+      <c r="Q8" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="Q8" s="23" t="s">
+      <c r="R8" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="R8" s="23" t="s">
+      <c r="S8" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="S8" s="23" t="s">
+      <c r="T8" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="T8" s="23" t="s">
+      <c r="U8" s="23" t="s">
         <v>82</v>
-      </c>
-      <c r="U8" s="23" t="s">
-        <v>83</v>
       </c>
       <c r="V8" s="23">
         <v>323277</v>
       </c>
       <c r="W8" s="25" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="X8" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y8" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="Y8" s="23" t="s">
+      <c r="Z8" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="Z8" s="23" t="s">
+      <c r="AA8" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB8" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC8" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="AD8" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="AA8" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="AB8" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="AC8" s="23" t="s">
-        <v>82</v>
-      </c>
-      <c r="AD8" s="23" t="s">
+      <c r="AE8" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="AE8" s="23" t="s">
+      <c r="AF8" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="AF8" s="23" t="s">
-        <v>90</v>
-      </c>
       <c r="AG8" s="23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AH8" s="23"/>
       <c r="AI8" s="23"/>
       <c r="AJ8" s="23"/>
       <c r="AK8" s="23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AL8" s="23"/>
       <c r="AM8" s="23"/>
@@ -2775,7 +2775,7 @@
       <c r="AX8" s="23"/>
       <c r="AY8" s="23"/>
       <c r="AZ8" s="23" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="BA8" s="23">
         <v>1</v>
@@ -2784,13 +2784,13 @@
         <v>250</v>
       </c>
       <c r="BC8" s="23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="BD8" s="23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="BE8" s="27" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="BF8" s="23">
         <v>10</v>
@@ -2802,21 +2802,21 @@
         <v>10</v>
       </c>
       <c r="BI8" s="23" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="BJ8" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="BK8" s="23" t="s">
         <v>102</v>
-      </c>
-      <c r="BK8" s="23" t="s">
-        <v>103</v>
       </c>
       <c r="BL8" s="23"/>
       <c r="BM8" s="23"/>
       <c r="BN8" s="23" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="BO8" s="26" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="BP8" s="22"/>
       <c r="BQ8" s="22"/>
@@ -2834,100 +2834,100 @@
       <c r="B9" s="48"/>
       <c r="C9" s="23"/>
       <c r="D9" s="24" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F9" s="23">
         <v>323284</v>
       </c>
       <c r="G9" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="H9" s="23" t="s">
         <v>123</v>
       </c>
-      <c r="H9" s="23" t="s">
-        <v>124</v>
-      </c>
       <c r="I9" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J9" s="23">
         <v>17</v>
       </c>
       <c r="K9" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="L9" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="L9" s="25" t="s">
+      <c r="M9" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="M9" s="25" t="s">
+      <c r="N9" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="N9" s="23" t="s">
+      <c r="O9" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="O9" s="23" t="s">
+      <c r="P9" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="P9" s="23" t="s">
+      <c r="Q9" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="Q9" s="23" t="s">
+      <c r="R9" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="R9" s="23" t="s">
+      <c r="S9" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="S9" s="23" t="s">
+      <c r="T9" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="T9" s="23" t="s">
+      <c r="U9" s="23" t="s">
         <v>82</v>
-      </c>
-      <c r="U9" s="23" t="s">
-        <v>83</v>
       </c>
       <c r="V9" s="23">
         <v>323284</v>
       </c>
       <c r="W9" s="25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="X9" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y9" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="Y9" s="23" t="s">
+      <c r="Z9" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="Z9" s="23" t="s">
+      <c r="AA9" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB9" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC9" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="AD9" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="AA9" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="AB9" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="AC9" s="23" t="s">
-        <v>82</v>
-      </c>
-      <c r="AD9" s="23" t="s">
+      <c r="AE9" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="AE9" s="23" t="s">
+      <c r="AF9" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="AF9" s="23" t="s">
-        <v>90</v>
-      </c>
       <c r="AG9" s="23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AH9" s="23"/>
       <c r="AI9" s="23"/>
       <c r="AJ9" s="23"/>
       <c r="AK9" s="23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AL9" s="23"/>
       <c r="AM9" s="23"/>
@@ -2944,7 +2944,7 @@
       <c r="AX9" s="23"/>
       <c r="AY9" s="23"/>
       <c r="AZ9" s="23" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="BA9" s="23">
         <v>1</v>
@@ -2953,10 +2953,10 @@
         <v>250</v>
       </c>
       <c r="BC9" s="23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="BD9" s="23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="BE9" s="23">
         <v>17</v>
@@ -2971,21 +2971,21 @@
         <v>10</v>
       </c>
       <c r="BI9" s="23" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="BJ9" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="BK9" s="23" t="s">
         <v>102</v>
-      </c>
-      <c r="BK9" s="23" t="s">
-        <v>103</v>
       </c>
       <c r="BL9" s="23"/>
       <c r="BM9" s="23"/>
       <c r="BN9" s="23" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="BO9" s="26" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="BP9" s="22"/>
       <c r="BQ9" s="22"/>
@@ -3003,102 +3003,102 @@
       <c r="B10" s="48"/>
       <c r="C10" s="23"/>
       <c r="D10" s="24" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E10" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F10" s="23">
         <v>323309</v>
       </c>
       <c r="G10" s="23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H10" s="23" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I10" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J10" s="23">
         <v>20</v>
       </c>
       <c r="K10" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="L10" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="L10" s="25" t="s">
+      <c r="M10" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="M10" s="25" t="s">
+      <c r="N10" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="N10" s="23" t="s">
+      <c r="O10" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="O10" s="23" t="s">
+      <c r="P10" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="P10" s="23" t="s">
+      <c r="Q10" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="Q10" s="23" t="s">
+      <c r="R10" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="R10" s="23" t="s">
+      <c r="S10" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="S10" s="23" t="s">
+      <c r="T10" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="T10" s="23" t="s">
+      <c r="U10" s="23" t="s">
         <v>82</v>
-      </c>
-      <c r="U10" s="23" t="s">
-        <v>83</v>
       </c>
       <c r="V10" s="23">
         <v>323309</v>
       </c>
       <c r="W10" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="X10" s="23" t="s">
         <v>126</v>
       </c>
-      <c r="X10" s="23" t="s">
+      <c r="Y10" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="Y10" s="23" t="s">
+      <c r="Z10" s="23" t="s">
         <v>128</v>
       </c>
-      <c r="Z10" s="23" t="s">
-        <v>129</v>
-      </c>
       <c r="AA10" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB10" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC10" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="AB10" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="AC10" s="23" t="s">
-        <v>82</v>
-      </c>
       <c r="AD10" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE10" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="AE10" s="23" t="s">
+      <c r="AF10" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="AF10" s="23" t="s">
-        <v>90</v>
-      </c>
       <c r="AG10" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="AH10" s="23" t="s">
         <v>81</v>
-      </c>
-      <c r="AH10" s="23" t="s">
-        <v>82</v>
       </c>
       <c r="AI10" s="23"/>
       <c r="AJ10" s="23"/>
       <c r="AK10" s="23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AL10" s="23"/>
       <c r="AM10" s="23"/>
@@ -3115,7 +3115,7 @@
       <c r="AX10" s="23"/>
       <c r="AY10" s="23"/>
       <c r="AZ10" s="23" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="BA10" s="23">
         <v>1</v>
@@ -3124,10 +3124,10 @@
         <v>250</v>
       </c>
       <c r="BC10" s="23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="BD10" s="23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="BE10" s="23">
         <v>20</v>
@@ -3142,21 +3142,21 @@
         <v>10</v>
       </c>
       <c r="BI10" s="23" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="BJ10" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="BK10" s="23" t="s">
         <v>102</v>
-      </c>
-      <c r="BK10" s="23" t="s">
-        <v>103</v>
       </c>
       <c r="BL10" s="23"/>
       <c r="BM10" s="23"/>
       <c r="BN10" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="BO10" s="26" t="s">
         <v>104</v>
-      </c>
-      <c r="BO10" s="26" t="s">
-        <v>105</v>
       </c>
       <c r="BP10" s="22"/>
       <c r="BQ10" s="22"/>
@@ -3174,100 +3174,100 @@
       <c r="B11" s="48"/>
       <c r="C11" s="23"/>
       <c r="D11" s="24" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E11" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F11" s="23">
         <v>323331</v>
       </c>
       <c r="G11" s="23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H11" s="23" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I11" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J11" s="23">
         <v>9</v>
       </c>
       <c r="K11" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="L11" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="L11" s="25" t="s">
+      <c r="M11" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="M11" s="25" t="s">
+      <c r="N11" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="N11" s="23" t="s">
+      <c r="O11" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="O11" s="23" t="s">
+      <c r="P11" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="P11" s="23" t="s">
+      <c r="Q11" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="Q11" s="23" t="s">
+      <c r="R11" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="R11" s="23" t="s">
+      <c r="S11" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="S11" s="23" t="s">
+      <c r="T11" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="T11" s="23" t="s">
+      <c r="U11" s="23" t="s">
         <v>82</v>
-      </c>
-      <c r="U11" s="23" t="s">
-        <v>83</v>
       </c>
       <c r="V11" s="23">
         <v>323331</v>
       </c>
       <c r="W11" s="25" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="X11" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="Y11" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="Y11" s="23" t="s">
+      <c r="Z11" s="23" t="s">
         <v>110</v>
       </c>
-      <c r="Z11" s="23" t="s">
-        <v>111</v>
-      </c>
       <c r="AA11" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB11" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC11" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="AB11" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="AC11" s="23" t="s">
-        <v>82</v>
-      </c>
       <c r="AD11" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE11" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="AE11" s="23" t="s">
+      <c r="AF11" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="AF11" s="23" t="s">
-        <v>90</v>
-      </c>
       <c r="AG11" s="23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AH11" s="23"/>
       <c r="AI11" s="23"/>
       <c r="AJ11" s="23"/>
       <c r="AK11" s="23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AL11" s="23"/>
       <c r="AM11" s="23"/>
@@ -3284,7 +3284,7 @@
       <c r="AX11" s="23"/>
       <c r="AY11" s="23"/>
       <c r="AZ11" s="23" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="BA11" s="23">
         <v>1</v>
@@ -3293,10 +3293,10 @@
         <v>250</v>
       </c>
       <c r="BC11" s="23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="BD11" s="23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="BE11" s="23">
         <v>9</v>
@@ -3311,21 +3311,21 @@
         <v>20</v>
       </c>
       <c r="BI11" s="23" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="BJ11" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="BK11" s="23" t="s">
         <v>102</v>
-      </c>
-      <c r="BK11" s="23" t="s">
-        <v>103</v>
       </c>
       <c r="BL11" s="23"/>
       <c r="BM11" s="23"/>
       <c r="BN11" s="23" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="BO11" s="26" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="BP11" s="22"/>
       <c r="BQ11" s="22"/>
@@ -3343,102 +3343,102 @@
       <c r="B12" s="48"/>
       <c r="C12" s="23"/>
       <c r="D12" s="24" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E12" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F12" s="23">
         <v>323287</v>
       </c>
       <c r="G12" s="23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H12" s="23" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I12" s="36" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J12" s="40">
         <v>20</v>
       </c>
       <c r="K12" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="L12" s="42" t="s">
         <v>73</v>
       </c>
-      <c r="L12" s="42" t="s">
+      <c r="M12" s="42" t="s">
         <v>74</v>
       </c>
-      <c r="M12" s="42" t="s">
+      <c r="N12" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="N12" s="36" t="s">
+      <c r="O12" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="O12" s="36" t="s">
+      <c r="P12" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="P12" s="36" t="s">
+      <c r="Q12" s="36" t="s">
         <v>78</v>
       </c>
-      <c r="Q12" s="36" t="s">
+      <c r="R12" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="R12" s="36" t="s">
+      <c r="S12" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="S12" s="36" t="s">
+      <c r="T12" s="36" t="s">
         <v>81</v>
       </c>
-      <c r="T12" s="36" t="s">
+      <c r="U12" s="36" t="s">
         <v>82</v>
-      </c>
-      <c r="U12" s="36" t="s">
-        <v>83</v>
       </c>
       <c r="V12" s="36">
         <v>323287</v>
       </c>
       <c r="W12" s="42" t="s">
+        <v>132</v>
+      </c>
+      <c r="X12" s="36" t="s">
         <v>133</v>
       </c>
-      <c r="X12" s="36" t="s">
+      <c r="Y12" s="36" t="s">
         <v>134</v>
-      </c>
-      <c r="Y12" s="36" t="s">
-        <v>135</v>
       </c>
       <c r="Z12" s="36">
         <v>98003</v>
       </c>
       <c r="AA12" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB12" s="36" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC12" s="36" t="s">
         <v>81</v>
       </c>
-      <c r="AB12" s="36" t="s">
-        <v>76</v>
-      </c>
-      <c r="AC12" s="36" t="s">
-        <v>82</v>
-      </c>
       <c r="AD12" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE12" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="AE12" s="36" t="s">
+      <c r="AF12" s="36" t="s">
         <v>89</v>
       </c>
-      <c r="AF12" s="36" t="s">
-        <v>90</v>
-      </c>
       <c r="AG12" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="AH12" s="36" t="s">
         <v>81</v>
-      </c>
-      <c r="AH12" s="36" t="s">
-        <v>82</v>
       </c>
       <c r="AI12" s="36"/>
       <c r="AJ12" s="36"/>
       <c r="AK12" s="36" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AL12" s="36"/>
       <c r="AM12" s="36"/>
@@ -3455,7 +3455,7 @@
       <c r="AX12" s="36"/>
       <c r="AY12" s="36"/>
       <c r="AZ12" s="36" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="BA12" s="36">
         <v>1</v>
@@ -3464,10 +3464,10 @@
         <v>250</v>
       </c>
       <c r="BC12" s="36" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="BD12" s="36" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="BE12" s="40">
         <v>20</v>
@@ -3482,21 +3482,21 @@
         <v>30</v>
       </c>
       <c r="BI12" s="36" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="BJ12" s="36" t="s">
+        <v>101</v>
+      </c>
+      <c r="BK12" s="36" t="s">
         <v>102</v>
-      </c>
-      <c r="BK12" s="36" t="s">
-        <v>103</v>
       </c>
       <c r="BL12" s="36"/>
       <c r="BM12" s="36"/>
       <c r="BN12" s="36" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="BO12" s="45" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="BP12" s="22"/>
       <c r="BQ12" s="22"/>
@@ -3512,98 +3512,98 @@
         <v>1</v>
       </c>
       <c r="B13" s="49" t="s">
+        <v>135</v>
+      </c>
+      <c r="C13" s="29" t="s">
         <v>136</v>
       </c>
-      <c r="C13" s="29" t="s">
+      <c r="D13" s="30" t="s">
         <v>137</v>
       </c>
-      <c r="D13" s="30" t="s">
-        <v>138</v>
-      </c>
       <c r="E13" s="31" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F13" s="29">
         <v>323351</v>
       </c>
       <c r="G13" s="29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H13" s="29" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I13" s="39" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J13" s="39">
         <v>105</v>
       </c>
       <c r="K13" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="L13" s="43" t="s">
         <v>73</v>
       </c>
-      <c r="L13" s="43" t="s">
+      <c r="M13" s="43" t="s">
         <v>74</v>
       </c>
-      <c r="M13" s="43" t="s">
+      <c r="N13" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="N13" s="39" t="s">
+      <c r="O13" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="O13" s="39" t="s">
+      <c r="P13" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="P13" s="39" t="s">
+      <c r="Q13" s="39" t="s">
         <v>78</v>
       </c>
-      <c r="Q13" s="39" t="s">
+      <c r="R13" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="R13" s="39" t="s">
+      <c r="S13" s="39" t="s">
         <v>80</v>
-      </c>
-      <c r="S13" s="39" t="s">
-        <v>81</v>
       </c>
       <c r="T13" s="29"/>
       <c r="U13" s="39" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="V13" s="39" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="W13" s="43" t="s">
+        <v>138</v>
+      </c>
+      <c r="X13" s="39" t="s">
         <v>139</v>
       </c>
-      <c r="X13" s="39" t="s">
+      <c r="Y13" s="39" t="s">
         <v>140</v>
-      </c>
-      <c r="Y13" s="39" t="s">
-        <v>141</v>
       </c>
       <c r="Z13" s="39">
         <v>30052</v>
       </c>
       <c r="AA13" s="39" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AB13" s="39" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AC13" s="39" t="b">
         <v>0</v>
       </c>
       <c r="AD13" s="39" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE13" s="39" t="s">
         <v>88</v>
       </c>
-      <c r="AE13" s="39" t="s">
+      <c r="AF13" s="39" t="s">
         <v>89</v>
       </c>
-      <c r="AF13" s="39" t="s">
-        <v>90</v>
-      </c>
       <c r="AG13" s="39" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AH13" s="39"/>
       <c r="AI13" s="39"/>
@@ -3624,7 +3624,7 @@
       <c r="AX13" s="39"/>
       <c r="AY13" s="39"/>
       <c r="AZ13" s="39" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="BA13" s="39">
         <v>1</v>
@@ -3633,10 +3633,10 @@
         <v>250</v>
       </c>
       <c r="BC13" s="39" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="BD13" s="39" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="BE13" s="39">
         <v>105</v>
@@ -3651,25 +3651,25 @@
         <v>20</v>
       </c>
       <c r="BI13" s="39" t="s">
+        <v>111</v>
+      </c>
+      <c r="BJ13" s="39" t="s">
+        <v>101</v>
+      </c>
+      <c r="BK13" s="39" t="s">
+        <v>102</v>
+      </c>
+      <c r="BL13" s="39" t="s">
+        <v>141</v>
+      </c>
+      <c r="BM13" s="39" t="s">
+        <v>142</v>
+      </c>
+      <c r="BN13" s="39" t="s">
+        <v>103</v>
+      </c>
+      <c r="BO13" s="46" t="s">
         <v>112</v>
-      </c>
-      <c r="BJ13" s="39" t="s">
-        <v>102</v>
-      </c>
-      <c r="BK13" s="39" t="s">
-        <v>103</v>
-      </c>
-      <c r="BL13" s="39" t="s">
-        <v>142</v>
-      </c>
-      <c r="BM13" s="39" t="s">
-        <v>143</v>
-      </c>
-      <c r="BN13" s="39" t="s">
-        <v>104</v>
-      </c>
-      <c r="BO13" s="46" t="s">
-        <v>113</v>
       </c>
       <c r="BP13" s="22"/>
       <c r="BQ13" s="22"/>
@@ -3686,96 +3686,96 @@
       </c>
       <c r="B14" s="49"/>
       <c r="C14" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="D14" s="30" t="s">
         <v>144</v>
       </c>
-      <c r="D14" s="30" t="s">
-        <v>145</v>
-      </c>
       <c r="E14" s="31" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F14" s="29">
         <v>323396</v>
       </c>
       <c r="G14" s="29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H14" s="29" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I14" s="29" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J14" s="29">
         <v>500</v>
       </c>
       <c r="K14" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="L14" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="L14" s="31" t="s">
+      <c r="M14" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="M14" s="31" t="s">
+      <c r="N14" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="N14" s="29" t="s">
+      <c r="O14" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="O14" s="29" t="s">
+      <c r="P14" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="P14" s="29" t="s">
+      <c r="Q14" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="Q14" s="29" t="s">
+      <c r="R14" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="R14" s="29" t="s">
+      <c r="S14" s="29" t="s">
         <v>80</v>
-      </c>
-      <c r="S14" s="29" t="s">
-        <v>81</v>
       </c>
       <c r="T14" s="29"/>
       <c r="U14" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="V14" s="29">
         <v>323396</v>
       </c>
       <c r="W14" s="31" t="s">
+        <v>146</v>
+      </c>
+      <c r="X14" s="29" t="s">
         <v>147</v>
       </c>
-      <c r="X14" s="29" t="s">
+      <c r="Y14" s="29" t="s">
         <v>148</v>
       </c>
-      <c r="Y14" s="29" t="s">
+      <c r="Z14" s="29" t="s">
         <v>149</v>
       </c>
-      <c r="Z14" s="29" t="s">
-        <v>150</v>
-      </c>
       <c r="AA14" s="29" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AB14" s="29">
         <v>9012633035</v>
       </c>
       <c r="AC14" s="29"/>
       <c r="AD14" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE14" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="AE14" s="29" t="s">
-        <v>89</v>
-      </c>
       <c r="AF14" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="AG14" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="AH14" s="29" t="s">
         <v>151</v>
-      </c>
-      <c r="AG14" s="29" t="s">
-        <v>81</v>
-      </c>
-      <c r="AH14" s="29" t="s">
-        <v>152</v>
       </c>
       <c r="AI14" s="29"/>
       <c r="AJ14" s="29"/>
@@ -3795,7 +3795,7 @@
       <c r="AX14" s="29"/>
       <c r="AY14" s="29"/>
       <c r="AZ14" s="29" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="BA14" s="29">
         <v>1</v>
@@ -3804,10 +3804,10 @@
         <v>7000</v>
       </c>
       <c r="BC14" s="29" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="BD14" s="29" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="BE14" s="29">
         <v>151</v>
@@ -3822,25 +3822,25 @@
         <v>40</v>
       </c>
       <c r="BI14" s="29" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="BJ14" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="BK14" s="29" t="s">
         <v>102</v>
       </c>
-      <c r="BK14" s="29" t="s">
+      <c r="BL14" s="29" t="s">
+        <v>141</v>
+      </c>
+      <c r="BM14" s="29" t="s">
+        <v>157</v>
+      </c>
+      <c r="BN14" s="29" t="s">
         <v>103</v>
       </c>
-      <c r="BL14" s="29" t="s">
-        <v>142</v>
-      </c>
-      <c r="BM14" s="29" t="s">
-        <v>158</v>
-      </c>
-      <c r="BN14" s="29" t="s">
+      <c r="BO14" s="32" t="s">
         <v>104</v>
-      </c>
-      <c r="BO14" s="32" t="s">
-        <v>105</v>
       </c>
       <c r="BP14" s="22"/>
       <c r="BQ14" s="22"/>
@@ -3857,144 +3857,144 @@
       </c>
       <c r="B15" s="50"/>
       <c r="C15" s="33" t="s">
+        <v>152</v>
+      </c>
+      <c r="D15" s="34" t="s">
         <v>153</v>
       </c>
-      <c r="D15" s="34" t="s">
-        <v>154</v>
-      </c>
       <c r="E15" s="35" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F15" s="33">
         <v>323365</v>
       </c>
       <c r="G15" s="33" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H15" s="33" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I15" s="33" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J15" s="33">
         <v>10</v>
       </c>
       <c r="K15" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="L15" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="L15" s="35" t="s">
+      <c r="M15" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="M15" s="35" t="s">
+      <c r="N15" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="N15" s="33" t="s">
+      <c r="O15" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="O15" s="33" t="s">
+      <c r="P15" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="P15" s="33" t="s">
+      <c r="Q15" s="33" t="s">
         <v>78</v>
       </c>
-      <c r="Q15" s="33" t="s">
+      <c r="R15" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="R15" s="33" t="s">
+      <c r="S15" s="33" t="s">
         <v>80</v>
-      </c>
-      <c r="S15" s="33" t="s">
-        <v>81</v>
       </c>
       <c r="T15" s="33"/>
       <c r="U15" s="33" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="V15" s="33" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="W15" s="35" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="X15" s="33" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="Y15" s="33" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="Z15" s="33">
         <v>99202</v>
       </c>
       <c r="AA15" s="33" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AB15" s="33" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AC15" s="33" t="b">
         <v>0</v>
       </c>
       <c r="AD15" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE15" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="AE15" s="33" t="s">
+      <c r="AF15" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="AF15" s="33" t="s">
-        <v>90</v>
-      </c>
       <c r="AG15" s="33" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AH15" s="33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AI15" s="33"/>
       <c r="AJ15" s="33" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AK15" s="33">
         <v>100</v>
       </c>
       <c r="AL15" s="33"/>
       <c r="AM15" s="33" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AN15" s="33" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="AO15" s="33">
         <v>123456789</v>
       </c>
       <c r="AP15" s="33" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AQ15" s="33"/>
       <c r="AR15" s="33" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AS15" s="33">
         <v>3305551234</v>
       </c>
       <c r="AT15" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="AU15" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="AU15" s="33" t="s">
+      <c r="AV15" s="33" t="s">
         <v>78</v>
       </c>
-      <c r="AV15" s="33" t="s">
+      <c r="AW15" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="AW15" s="33" t="s">
+      <c r="AX15" s="33" t="s">
         <v>80</v>
-      </c>
-      <c r="AX15" s="33" t="s">
-        <v>81</v>
       </c>
       <c r="AY15" s="33"/>
       <c r="AZ15" s="33" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="BA15" s="33">
         <v>1</v>
@@ -4003,10 +4003,10 @@
         <v>7000</v>
       </c>
       <c r="BC15" s="33" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="BD15" s="33" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="BE15" s="33">
         <v>10</v>
@@ -4021,21 +4021,21 @@
         <v>20</v>
       </c>
       <c r="BI15" s="33" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="BJ15" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="BK15" s="33" t="s">
         <v>102</v>
-      </c>
-      <c r="BK15" s="33" t="s">
-        <v>103</v>
       </c>
       <c r="BL15" s="33"/>
       <c r="BM15" s="33"/>
       <c r="BN15" s="33" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="BO15" s="37" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="BP15" s="22"/>
       <c r="BQ15" s="22"/>

</xml_diff>

<commit_message>
TP#20088: Fixed 7 cases that came back.
</commit_message>
<xml_diff>
--- a/Code/ShipWorks.Tests.Integration/DataSources/FedExAll/US Exp Dom-Alcohol.xlsx
+++ b/Code/ShipWorks.Tests.Integration/DataSources/FedExAll/US Exp Dom-Alcohol.xlsx
@@ -1313,7 +1313,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BO15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:XFD14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>